<commit_message>
Changed ISRIC2011 from raster to list of rasters. ISRIC2011$main contains main class info. Broke apart read_P_ISRIC into various functions. Improved notebooks encapsultaing plot code into nb_code for formatting in notebook render. Added plot_P_scales, and related functions. Removed some external data. Update documentation accordingly. TODO: extract coordinates from Romero-Navarro 2017
</commit_message>
<xml_diff>
--- a/inst/extdata/P_retention_class.xlsx
+++ b/inst/extdata/P_retention_class.xlsx
@@ -12,7 +12,7 @@
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$18</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$K$18</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$I$18</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t xml:space="preserve">main</t>
   </si>
@@ -38,9 +38,6 @@
     <t xml:space="preserve">ascending</t>
   </si>
   <si>
-    <t xml:space="preserve">descending</t>
-  </si>
-  <si>
     <t xml:space="preserve">r</t>
   </si>
   <si>
@@ -65,6 +62,78 @@
     <t xml:space="preserve">Oceans/Inland waters</t>
   </si>
   <si>
+    <t xml:space="preserve">GL1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Glaciers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RK1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;75% Rock Outcrops</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RK2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">50-75% Rock Outcrops</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lo1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;75% Low</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lo2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">50-75% Low</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lo3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25-50% Low</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mo2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">50-75% Moderate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mo1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;75% Moderate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mo3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25-50% Moderate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hi3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25-50% High</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hi2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">50-75% High</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hi1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;75% High</t>
+  </si>
+  <si>
     <t xml:space="preserve">VH3</t>
   </si>
   <si>
@@ -81,78 +150,6 @@
   </si>
   <si>
     <t xml:space="preserve">&gt;75% Very High</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RK2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">50-75% Rock Outcrops</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RK1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&gt;75% Rock Outcrops</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mo3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25-50% Moderate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mo2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">50-75% Moderate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mo1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&gt;75% Moderate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lo3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25-50% Low</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lo2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">50-75% Low</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lo1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&gt;75% Low</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hi3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25-50% High</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hi2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">50-75% High</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hi1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&gt;75% High</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GL1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Glaciers</t>
   </si>
   <si>
     <t xml:space="preserve">NA</t>
@@ -260,30 +257,32 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:ALX18"/>
+  <dimension ref="A1:ALW18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="2" style="0" width="12.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="4.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="4.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="12.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="13.04"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="18.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="8.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="12.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="13.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="15" style="0" width="12.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="13.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="14.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="19" style="0" width="12.9"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="21" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="4.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="4.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.04"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="18.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="8.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="12.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="13.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="14" style="0" width="12.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="13.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="14.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="18" style="0" width="12.9"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="20" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -317,18 +316,15 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="ALX1" s="1"/>
+      <c r="ALW1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="0" t="s">
-        <v>12</v>
-      </c>
       <c r="C2" s="0" t="n">
         <v>0</v>
       </c>
@@ -336,470 +332,422 @@
         <v>0</v>
       </c>
       <c r="E2" s="0" t="n">
-        <v>16</v>
+        <v>190</v>
       </c>
       <c r="F2" s="0" t="n">
-        <v>190</v>
+        <v>232</v>
       </c>
       <c r="G2" s="0" t="n">
-        <v>232</v>
+        <v>255</v>
       </c>
       <c r="H2" s="0" t="n">
-        <v>255</v>
-      </c>
-      <c r="I2" s="0" t="n">
         <v>17</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="0" t="s">
-        <v>14</v>
-      </c>
       <c r="C3" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="D3" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D3" s="0" t="n">
-        <v>13</v>
-      </c>
       <c r="E3" s="0" t="n">
-        <v>3</v>
+        <v>225</v>
       </c>
       <c r="F3" s="0" t="n">
-        <v>255</v>
+        <v>225</v>
       </c>
       <c r="G3" s="0" t="n">
-        <v>127</v>
+        <v>225</v>
       </c>
       <c r="H3" s="0" t="n">
-        <v>127</v>
-      </c>
-      <c r="I3" s="0" t="n">
-        <v>16</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="0" t="s">
-        <v>16</v>
-      </c>
       <c r="C4" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="D4" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="D4" s="0" t="n">
-        <v>14</v>
-      </c>
       <c r="E4" s="0" t="n">
-        <v>2</v>
+        <v>130</v>
       </c>
       <c r="F4" s="0" t="n">
-        <v>230</v>
+        <v>130</v>
       </c>
       <c r="G4" s="0" t="n">
-        <v>0</v>
+        <v>130</v>
       </c>
       <c r="H4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I4" s="0" t="n">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="0" t="s">
-        <v>18</v>
-      </c>
       <c r="C5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="D5" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="D5" s="0" t="n">
-        <v>15</v>
-      </c>
       <c r="E5" s="0" t="n">
-        <v>1</v>
+        <v>156</v>
       </c>
       <c r="F5" s="0" t="n">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="G5" s="0" t="n">
-        <v>0</v>
+        <v>156</v>
       </c>
       <c r="H5" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I5" s="0" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="C6" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="D6" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="D6" s="0" t="n">
-        <v>3</v>
-      </c>
       <c r="E6" s="0" t="n">
-        <v>14</v>
+        <v>152</v>
       </c>
       <c r="F6" s="0" t="n">
-        <v>156</v>
+        <v>230</v>
       </c>
       <c r="G6" s="0" t="n">
-        <v>156</v>
+        <v>0</v>
       </c>
       <c r="H6" s="0" t="n">
-        <v>156</v>
-      </c>
-      <c r="I6" s="0" t="n">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="0" t="s">
-        <v>22</v>
-      </c>
       <c r="C7" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="D7" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="D7" s="0" t="n">
-        <v>2</v>
-      </c>
       <c r="E7" s="0" t="n">
-        <v>13</v>
+        <v>170</v>
       </c>
       <c r="F7" s="0" t="n">
-        <v>130</v>
+        <v>255</v>
       </c>
       <c r="G7" s="0" t="n">
-        <v>130</v>
+        <v>0</v>
       </c>
       <c r="H7" s="0" t="n">
-        <v>130</v>
-      </c>
-      <c r="I7" s="0" t="n">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="0" t="s">
-        <v>24</v>
-      </c>
       <c r="C8" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="D8" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="D8" s="0" t="n">
-        <v>7</v>
-      </c>
       <c r="E8" s="0" t="n">
-        <v>9</v>
+        <v>209</v>
       </c>
       <c r="F8" s="0" t="n">
         <v>255</v>
       </c>
       <c r="G8" s="0" t="n">
-        <v>235</v>
+        <v>115</v>
       </c>
       <c r="H8" s="0" t="n">
-        <v>190</v>
-      </c>
-      <c r="I8" s="0" t="n">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="0" t="s">
         <v>25</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>26</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>7</v>
       </c>
       <c r="D9" s="0" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E9" s="0" t="n">
-        <v>8</v>
+        <v>255</v>
       </c>
       <c r="F9" s="0" t="n">
-        <v>255</v>
+        <v>235</v>
       </c>
       <c r="G9" s="0" t="n">
-        <v>235</v>
+        <v>175</v>
       </c>
       <c r="H9" s="0" t="n">
-        <v>175</v>
-      </c>
-      <c r="I9" s="0" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="0" t="s">
         <v>27</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>28</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>8</v>
       </c>
       <c r="D10" s="0" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E10" s="0" t="n">
-        <v>7</v>
+        <v>255</v>
       </c>
       <c r="F10" s="0" t="n">
-        <v>255</v>
+        <v>211</v>
       </c>
       <c r="G10" s="0" t="n">
-        <v>211</v>
+        <v>127</v>
       </c>
       <c r="H10" s="0" t="n">
-        <v>127</v>
-      </c>
-      <c r="I10" s="0" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="0" t="s">
-        <v>30</v>
-      </c>
       <c r="C11" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="D11" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="D11" s="0" t="n">
-        <v>6</v>
-      </c>
       <c r="E11" s="0" t="n">
-        <v>10</v>
+        <v>255</v>
       </c>
       <c r="F11" s="0" t="n">
-        <v>209</v>
+        <v>235</v>
       </c>
       <c r="G11" s="0" t="n">
-        <v>255</v>
+        <v>190</v>
       </c>
       <c r="H11" s="0" t="n">
-        <v>115</v>
-      </c>
-      <c r="I11" s="0" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="0" t="s">
-        <v>32</v>
-      </c>
       <c r="C12" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="D12" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="D12" s="0" t="n">
+      <c r="E12" s="0" t="n">
+        <v>215</v>
+      </c>
+      <c r="F12" s="0" t="n">
+        <v>158</v>
+      </c>
+      <c r="G12" s="0" t="n">
+        <v>158</v>
+      </c>
+      <c r="H12" s="0" t="n">
         <v>5</v>
-      </c>
-      <c r="E12" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="F12" s="0" t="n">
-        <v>170</v>
-      </c>
-      <c r="G12" s="0" t="n">
-        <v>255</v>
-      </c>
-      <c r="H12" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I12" s="0" t="n">
-        <v>7</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="B13" s="0" t="s">
-        <v>34</v>
-      </c>
       <c r="C13" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="D13" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="D13" s="0" t="n">
+      <c r="E13" s="0" t="n">
+        <v>245</v>
+      </c>
+      <c r="F13" s="0" t="n">
+        <v>122</v>
+      </c>
+      <c r="G13" s="0" t="n">
+        <v>122</v>
+      </c>
+      <c r="H13" s="0" t="n">
         <v>4</v>
-      </c>
-      <c r="E13" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="F13" s="0" t="n">
-        <v>152</v>
-      </c>
-      <c r="G13" s="0" t="n">
-        <v>230</v>
-      </c>
-      <c r="H13" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I13" s="0" t="n">
-        <v>6</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="B14" s="0" t="s">
-        <v>36</v>
-      </c>
       <c r="C14" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="D14" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="D14" s="0" t="n">
-        <v>10</v>
-      </c>
       <c r="E14" s="0" t="n">
-        <v>6</v>
+        <v>205</v>
       </c>
       <c r="F14" s="0" t="n">
-        <v>215</v>
+        <v>102</v>
       </c>
       <c r="G14" s="0" t="n">
-        <v>158</v>
+        <v>102</v>
       </c>
       <c r="H14" s="0" t="n">
-        <v>158</v>
-      </c>
-      <c r="I14" s="0" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="B15" s="0" t="s">
-        <v>38</v>
-      </c>
       <c r="C15" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D15" s="0" t="n">
         <v>13</v>
       </c>
-      <c r="D15" s="0" t="n">
-        <v>11</v>
-      </c>
       <c r="E15" s="0" t="n">
-        <v>5</v>
+        <v>255</v>
       </c>
       <c r="F15" s="0" t="n">
-        <v>245</v>
+        <v>127</v>
       </c>
       <c r="G15" s="0" t="n">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="H15" s="0" t="n">
-        <v>122</v>
-      </c>
-      <c r="I15" s="0" t="n">
-        <v>4</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="B16" s="0" t="s">
-        <v>40</v>
-      </c>
       <c r="C16" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D16" s="0" t="n">
         <v>14</v>
       </c>
-      <c r="D16" s="0" t="n">
-        <v>12</v>
-      </c>
       <c r="E16" s="0" t="n">
-        <v>4</v>
+        <v>230</v>
       </c>
       <c r="F16" s="0" t="n">
-        <v>205</v>
+        <v>0</v>
       </c>
       <c r="G16" s="0" t="n">
-        <v>102</v>
+        <v>0</v>
       </c>
       <c r="H16" s="0" t="n">
-        <v>102</v>
-      </c>
-      <c r="I16" s="0" t="n">
-        <v>3</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B17" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="B17" s="0" t="s">
-        <v>42</v>
-      </c>
       <c r="C17" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D17" s="0" t="n">
         <v>15</v>
       </c>
-      <c r="D17" s="0" t="n">
-        <v>1</v>
-      </c>
       <c r="E17" s="0" t="n">
-        <v>15</v>
+        <v>168</v>
       </c>
       <c r="F17" s="0" t="n">
-        <v>225</v>
+        <v>0</v>
       </c>
       <c r="G17" s="0" t="n">
-        <v>225</v>
+        <v>0</v>
       </c>
       <c r="H17" s="0" t="n">
-        <v>225</v>
-      </c>
-      <c r="I17" s="0" t="n">
-        <v>2</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="0" t="s">
-        <v>43</v>
+        <v>42</v>
+      </c>
+      <c r="E18" s="0" t="n">
+        <v>48</v>
       </c>
       <c r="F18" s="0" t="n">
-        <v>48</v>
+        <v>196</v>
       </c>
       <c r="G18" s="0" t="n">
-        <v>196</v>
+        <v>46</v>
       </c>
       <c r="H18" s="0" t="n">
-        <v>46</v>
-      </c>
-      <c r="I18" s="0" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>